<commit_message>
finished figuring out function to report on response variables
</commit_message>
<xml_diff>
--- a/simulation/documents/mock_master.xlsx
+++ b/simulation/documents/mock_master.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23860" windowHeight="14780" tabRatio="500"/>
+    <workbookView xWindow="26440" yWindow="0" windowWidth="23860" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="community level" sheetId="1" r:id="rId1"/>
+    <sheet name="time step level" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -593,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
@@ -1325,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>